<commit_message>
Corection bug shooter + Ajout chargement du tout les monstre
</commit_message>
<xml_diff>
--- a/sources/Outiles/MobMap/AllMobe.xlsx
+++ b/sources/Outiles/MobMap/AllMobe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat_wfpn4na\Documents\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\MobMap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat_wfpn4na\Documents\GitHub\Jeu-Dzarian-Miniquoinquoin\sources\Outiles\MobMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E56D13-6060-424E-A4AD-ECF94C572F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4EED30-1F54-4D95-BA41-5E50A19487A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30780" yWindow="120" windowWidth="20820" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1140" windowWidth="21600" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -1074,15 +1074,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1091,24 +1082,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1130,14 +1103,41 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1497,10 +1497,10 @@
   <dimension ref="A1:BQ50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomRight" activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,59 +1530,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="8" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="8" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="8" t="s">
+      <c r="L1" s="35"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="8" t="s">
+      <c r="O1" s="35"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="8" t="s">
+      <c r="R1" s="35"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="9"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="8" t="s">
+      <c r="U1" s="35"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="10"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="36"/>
     </row>
     <row r="2" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
+      <c r="A2" s="15"/>
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1591,7 +1591,7 @@
       <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="6" t="s">
@@ -1600,7 +1600,7 @@
       <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="6" t="s">
@@ -1609,7 +1609,7 @@
       <c r="L2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="N2" s="6" t="s">
@@ -1618,7 +1618,7 @@
       <c r="O2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="Q2" s="6" t="s">
@@ -1627,7 +1627,7 @@
       <c r="R2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="T2" s="6" t="s">
@@ -1636,7 +1636,7 @@
       <c r="U2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="W2" s="6" t="s">
@@ -1645,7 +1645,7 @@
       <c r="X2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Y2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="Z2" s="5"/>
@@ -1694,50 +1694,50 @@
       <c r="BQ2" s="5"/>
     </row>
     <row r="3" spans="1:69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="32">
         <v>1</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="14">
         <v>1</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="14">
         <v>1</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="14">
         <v>2</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="14">
         <v>1</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="Q3" s="1" t="s">
@@ -1746,25 +1746,25 @@
       <c r="R3" s="3">
         <v>1</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="U3" s="34">
+      <c r="U3" s="32">
         <v>1</v>
       </c>
-      <c r="V3" s="35" t="s">
+      <c r="V3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="W3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="X3" s="29">
+      <c r="X3" s="20">
         <v>1</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Y3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="Z3" s="5"/>
@@ -1813,19 +1813,19 @@
       <c r="BQ3" s="5"/>
     </row>
     <row r="4" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1834,44 +1834,44 @@
       <c r="I4" s="3">
         <v>2</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="19">
+      <c r="L4" s="26">
         <v>1</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O4" s="19">
+      <c r="O4" s="26">
         <v>1</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R4" s="19">
+      <c r="R4" s="26">
         <v>1</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="S4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="23"/>
-      <c r="V4" s="24"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="29"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="12"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="9"/>
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
@@ -1918,14 +1918,14 @@
       <c r="BQ4" s="5"/>
     </row>
     <row r="5" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1934,39 +1934,39 @@
       <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="12"/>
+      <c r="J5" s="9"/>
       <c r="K5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="29"/>
       <c r="N5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="22"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="31"/>
       <c r="Q5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="21"/>
-      <c r="S5" s="22"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="31"/>
       <c r="T5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U5" s="19">
+      <c r="U5" s="26">
         <v>1</v>
       </c>
-      <c r="V5" s="20" t="s">
+      <c r="V5" s="28" t="s">
         <v>3</v>
       </c>
       <c r="W5" s="1"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="33"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="24"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
@@ -2013,55 +2013,55 @@
       <c r="BQ5" s="5"/>
     </row>
     <row r="6" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="12" t="s">
         <v>89</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="3">
         <v>2</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I6" s="3">
         <v>2</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="15"/>
+      <c r="K6" s="12"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="15" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="15" t="s">
+      <c r="O6" s="27"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="23"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="15" t="s">
+      <c r="R6" s="27"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="U6" s="21"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="31"/>
-      <c r="Y6" s="33"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="24"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
@@ -2108,14 +2108,14 @@
       <c r="BQ6" s="5"/>
     </row>
     <row r="7" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -2124,47 +2124,47 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="12"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="L7" s="3">
         <v>1</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="12" t="s">
         <v>30</v>
       </c>
       <c r="O7" s="3">
         <v>2</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="P7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="19">
+      <c r="R7" s="26">
         <v>2</v>
       </c>
-      <c r="S7" s="20" t="s">
+      <c r="S7" s="28" t="s">
         <v>3</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="U7" s="21"/>
-      <c r="V7" s="22"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="31"/>
       <c r="W7" s="1"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="33"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="24"/>
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
@@ -2211,47 +2211,47 @@
       <c r="BQ7" s="5"/>
     </row>
     <row r="8" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="12"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="26">
         <v>1</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="28" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="12"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="1"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="12"/>
+      <c r="M8" s="9"/>
       <c r="N8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="O8" s="3">
         <v>2</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="9" t="s">
         <v>2</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R8" s="23"/>
-      <c r="S8" s="24"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="29"/>
       <c r="T8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="U8" s="21"/>
-      <c r="V8" s="22"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="31"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="33"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="24"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
@@ -2298,25 +2298,25 @@
       <c r="BQ8" s="5"/>
     </row>
     <row r="9" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="1"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="12"/>
+      <c r="J9" s="9"/>
       <c r="K9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="26">
         <v>1</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="28" t="s">
         <v>3</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -2325,20 +2325,20 @@
       <c r="O9" s="3">
         <v>1</v>
       </c>
-      <c r="P9" s="12" t="s">
+      <c r="P9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="12"/>
+      <c r="S9" s="9"/>
       <c r="T9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="U9" s="21"/>
-      <c r="V9" s="22"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="31"/>
       <c r="W9" s="1"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="12"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="9"/>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
@@ -2385,47 +2385,47 @@
       <c r="BQ9" s="5"/>
     </row>
     <row r="10" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="1"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="1"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="12"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="26">
         <v>2</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="28" t="s">
         <v>3</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="12"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="29"/>
       <c r="N10" s="1" t="s">
         <v>47</v>
       </c>
       <c r="O10" s="3">
         <v>1</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="P10" s="9" t="s">
         <v>3</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="12"/>
+      <c r="S10" s="9"/>
       <c r="T10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U10" s="23"/>
-      <c r="V10" s="24"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="29"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="12"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="9"/>
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
@@ -2472,45 +2472,45 @@
       <c r="BQ10" s="5"/>
     </row>
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="26">
         <v>1</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="28" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="12"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="22"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="31"/>
       <c r="K11" s="1"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="12"/>
+      <c r="M11" s="9"/>
       <c r="N11" s="1" t="s">
         <v>69</v>
       </c>
       <c r="O11" s="3">
         <v>2</v>
       </c>
-      <c r="P11" s="12" t="s">
+      <c r="P11" s="9" t="s">
         <v>2</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="12"/>
+      <c r="S11" s="9"/>
       <c r="T11" s="1"/>
       <c r="U11" s="3"/>
-      <c r="V11" s="12"/>
+      <c r="V11" s="9"/>
       <c r="W11" s="1"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="12"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="9"/>
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
@@ -2557,288 +2557,288 @@
       <c r="BQ11" s="5"/>
     </row>
     <row r="12" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="12"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="29"/>
       <c r="K12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L12" s="26">
         <v>2</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="M12" s="28" t="s">
         <v>3</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="26">
         <v>1</v>
       </c>
-      <c r="P12" s="20" t="s">
+      <c r="P12" s="28" t="s">
         <v>3</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="12"/>
+      <c r="S12" s="9"/>
       <c r="T12" s="1"/>
       <c r="U12" s="3"/>
-      <c r="V12" s="12"/>
+      <c r="V12" s="9"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="12"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="9"/>
     </row>
     <row r="13" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="12"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="1"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="12"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="1"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="15" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31"/>
       <c r="N13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O13" s="23"/>
-      <c r="P13" s="24"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="29"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="12"/>
+      <c r="S13" s="9"/>
       <c r="T13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="U13" s="19">
+      <c r="U13" s="26">
         <v>1</v>
       </c>
-      <c r="V13" s="20" t="s">
+      <c r="V13" s="28" t="s">
         <v>3</v>
       </c>
       <c r="W13" s="1"/>
-      <c r="X13" s="30"/>
-      <c r="Y13" s="12"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="9"/>
     </row>
     <row r="14" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="12"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="1"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="12"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="1"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="12"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="24"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="29"/>
       <c r="N14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="26">
         <v>1</v>
       </c>
-      <c r="P14" s="20" t="s">
+      <c r="P14" s="28" t="s">
         <v>7</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="12"/>
+      <c r="S14" s="9"/>
       <c r="T14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="U14" s="23"/>
-      <c r="V14" s="24"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="29"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="30"/>
-      <c r="Y14" s="12"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="9"/>
     </row>
     <row r="15" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="12"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="1"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="12"/>
+      <c r="J15" s="9"/>
       <c r="K15" s="1"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="12"/>
+      <c r="M15" s="9"/>
       <c r="N15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="21"/>
-      <c r="P15" s="22"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="31"/>
       <c r="Q15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="R15" s="19">
+      <c r="R15" s="26">
         <v>2</v>
       </c>
-      <c r="S15" s="20" t="s">
+      <c r="S15" s="28" t="s">
         <v>3</v>
       </c>
       <c r="T15" s="1"/>
       <c r="U15" s="3"/>
-      <c r="V15" s="12"/>
+      <c r="V15" s="9"/>
       <c r="W15" s="1"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="12"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="9"/>
     </row>
     <row r="16" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="1"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="1"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="12"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="1"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="12"/>
+      <c r="M16" s="9"/>
       <c r="N16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O16" s="21"/>
-      <c r="P16" s="22"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="31"/>
       <c r="Q16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="23"/>
-      <c r="S16" s="24"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="29"/>
       <c r="T16" s="1"/>
       <c r="U16" s="3"/>
-      <c r="V16" s="12"/>
+      <c r="V16" s="9"/>
       <c r="W16" s="1"/>
-      <c r="X16" s="30"/>
-      <c r="Y16" s="12"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="9"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="1"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="12"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="1"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="12"/>
+      <c r="J17" s="9"/>
       <c r="K17" s="1"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="12"/>
+      <c r="M17" s="9"/>
       <c r="N17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O17" s="23"/>
-      <c r="P17" s="24"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="29"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="12"/>
+      <c r="S17" s="9"/>
       <c r="T17" s="1"/>
       <c r="U17" s="3"/>
-      <c r="V17" s="12"/>
+      <c r="V17" s="9"/>
       <c r="W17" s="1"/>
-      <c r="X17" s="30"/>
-      <c r="Y17" s="12"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="9"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="12"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="1"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="12"/>
+      <c r="J18" s="9"/>
       <c r="K18" s="1"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="12"/>
+      <c r="M18" s="9"/>
       <c r="N18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="26">
         <v>2</v>
       </c>
-      <c r="P18" s="20" t="s">
+      <c r="P18" s="28" t="s">
         <v>80</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="3"/>
-      <c r="S18" s="12"/>
+      <c r="S18" s="9"/>
       <c r="T18" s="1"/>
       <c r="U18" s="3"/>
-      <c r="V18" s="12"/>
+      <c r="V18" s="9"/>
       <c r="W18" s="1"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="12"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="9"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="12"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="1"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="12"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="1"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="12"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="1"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="12"/>
+      <c r="M19" s="9"/>
       <c r="N19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="23"/>
-      <c r="P19" s="24"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="29"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="12"/>
+      <c r="S19" s="9"/>
       <c r="T19" s="1"/>
       <c r="U19" s="3"/>
-      <c r="V19" s="12"/>
+      <c r="V19" s="9"/>
       <c r="W19" s="1"/>
-      <c r="X19" s="30"/>
-      <c r="Y19" s="12"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="9"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="3">
         <v>3</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="9" t="s">
         <v>36</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -2847,7 +2847,7 @@
       <c r="F20" s="3">
         <v>3</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="9" t="s">
         <v>64</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -2856,7 +2856,7 @@
       <c r="I20" s="3">
         <v>3</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J20" s="9" t="s">
         <v>64</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -2865,19 +2865,19 @@
       <c r="L20" s="3">
         <v>3</v>
       </c>
-      <c r="M20" s="12" t="s">
+      <c r="M20" s="9" t="s">
         <v>36</v>
       </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="28"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="19"/>
       <c r="Q20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="R20" s="3">
         <v>4</v>
       </c>
-      <c r="S20" s="12" t="s">
+      <c r="S20" s="9" t="s">
         <v>36</v>
       </c>
       <c r="T20" s="1" t="s">
@@ -2886,31 +2886,31 @@
       <c r="U20" s="3">
         <v>4</v>
       </c>
-      <c r="V20" s="12" t="s">
+      <c r="V20" s="9" t="s">
         <v>53</v>
       </c>
       <c r="W20" s="1"/>
-      <c r="X20" s="30"/>
-      <c r="Y20" s="12"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="9"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="12"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="1"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="12"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="1"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="12"/>
+      <c r="J21" s="9"/>
       <c r="K21" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L21" s="3">
         <v>3</v>
       </c>
-      <c r="M21" s="12" t="s">
+      <c r="M21" s="9" t="s">
         <v>36</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -2919,16 +2919,16 @@
       <c r="O21" s="3">
         <v>3</v>
       </c>
-      <c r="P21" s="12" t="s">
+      <c r="P21" s="9" t="s">
         <v>36</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="R21" s="19">
+      <c r="R21" s="26">
         <v>3</v>
       </c>
-      <c r="S21" s="20" t="s">
+      <c r="S21" s="28" t="s">
         <v>64</v>
       </c>
       <c r="T21" s="1" t="s">
@@ -2937,118 +2937,118 @@
       <c r="U21" s="3">
         <v>3</v>
       </c>
-      <c r="V21" s="12" t="s">
+      <c r="V21" s="9" t="s">
         <v>64</v>
       </c>
       <c r="W21" s="1"/>
-      <c r="X21" s="30"/>
-      <c r="Y21" s="12"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="9"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C22" s="3">
         <v>3</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="9" t="s">
         <v>36</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="12"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="1"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="12"/>
+      <c r="J22" s="9"/>
       <c r="K22" s="1"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="12"/>
+      <c r="M22" s="9"/>
       <c r="N22" s="1" t="s">
         <v>66</v>
       </c>
       <c r="O22" s="3">
         <v>4</v>
       </c>
-      <c r="P22" s="12" t="s">
+      <c r="P22" s="9" t="s">
         <v>36</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R22" s="21"/>
-      <c r="S22" s="22"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="31"/>
       <c r="T22" s="1"/>
       <c r="U22" s="3"/>
-      <c r="V22" s="12"/>
+      <c r="V22" s="9"/>
       <c r="W22" s="1"/>
-      <c r="X22" s="30"/>
-      <c r="Y22" s="12"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="9"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="26">
         <v>3</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="28" t="s">
         <v>64</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="12"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="1"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="12"/>
+      <c r="J23" s="9"/>
       <c r="K23" s="1"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="12"/>
+      <c r="M23" s="9"/>
       <c r="N23" s="1" t="s">
         <v>70</v>
       </c>
       <c r="O23" s="3">
         <v>5</v>
       </c>
-      <c r="P23" s="12" t="s">
+      <c r="P23" s="9" t="s">
         <v>64</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="R23" s="23"/>
-      <c r="S23" s="24"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="29"/>
       <c r="T23" s="1"/>
       <c r="U23" s="3"/>
-      <c r="V23" s="12"/>
+      <c r="V23" s="9"/>
       <c r="W23" s="1"/>
-      <c r="X23" s="30"/>
-      <c r="Y23" s="12"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="9"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="24"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="12"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="1"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="12"/>
+      <c r="J24" s="9"/>
       <c r="K24" s="1"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="12"/>
+      <c r="M24" s="9"/>
       <c r="N24" s="1" t="s">
         <v>72</v>
       </c>
       <c r="O24" s="3">
         <v>3</v>
       </c>
-      <c r="P24" s="12" t="s">
+      <c r="P24" s="9" t="s">
         <v>64</v>
       </c>
       <c r="Q24" s="1" t="s">
@@ -3057,764 +3057,728 @@
       <c r="R24" s="3">
         <v>2</v>
       </c>
-      <c r="S24" s="12" t="s">
+      <c r="S24" s="9" t="s">
         <v>64</v>
       </c>
       <c r="T24" s="1"/>
       <c r="U24" s="3"/>
-      <c r="V24" s="12"/>
+      <c r="V24" s="9"/>
       <c r="W24" s="1"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="12"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="9"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="12"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="12"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="1"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="12"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="1"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="12"/>
+      <c r="M25" s="9"/>
       <c r="N25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O25" s="19">
+      <c r="O25" s="26">
         <v>3</v>
       </c>
-      <c r="P25" s="20" t="s">
+      <c r="P25" s="28" t="s">
         <v>36</v>
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="3"/>
-      <c r="S25" s="12"/>
+      <c r="S25" s="9"/>
       <c r="T25" s="1"/>
       <c r="U25" s="3"/>
-      <c r="V25" s="12"/>
+      <c r="V25" s="9"/>
       <c r="W25" s="1"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="12"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="9"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="1"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="12"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="1"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="12"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="1"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="12"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="1"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="12"/>
+      <c r="M26" s="9"/>
       <c r="N26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="23"/>
-      <c r="P26" s="24"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="29"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="3"/>
-      <c r="S26" s="12"/>
+      <c r="S26" s="9"/>
       <c r="T26" s="1"/>
       <c r="U26" s="3"/>
-      <c r="V26" s="12"/>
+      <c r="V26" s="9"/>
       <c r="W26" s="1"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="12"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="9"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="1"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="12"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="1"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="12"/>
+      <c r="G27" s="9"/>
       <c r="H27" s="1"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="12"/>
+      <c r="J27" s="9"/>
       <c r="K27" s="1"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="12"/>
+      <c r="M27" s="9"/>
       <c r="N27" s="1"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="28"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="19"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="12"/>
+      <c r="S27" s="9"/>
       <c r="T27" s="1"/>
       <c r="U27" s="3"/>
-      <c r="V27" s="12"/>
+      <c r="V27" s="9"/>
       <c r="W27" s="1"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="12"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="9"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="1"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="12"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="1"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="12"/>
+      <c r="G28" s="9"/>
       <c r="H28" s="1"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="12"/>
+      <c r="J28" s="9"/>
       <c r="K28" s="1"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="12"/>
+      <c r="M28" s="9"/>
       <c r="N28" s="1"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="12"/>
+      <c r="P28" s="9"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="12"/>
+      <c r="S28" s="9"/>
       <c r="T28" s="1"/>
       <c r="U28" s="3"/>
-      <c r="V28" s="12"/>
+      <c r="V28" s="9"/>
       <c r="W28" s="1"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="12"/>
+      <c r="X28" s="21"/>
+      <c r="Y28" s="9"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="1"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="12"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="1"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="12"/>
+      <c r="G29" s="9"/>
       <c r="H29" s="1"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="12"/>
+      <c r="J29" s="9"/>
       <c r="K29" s="1"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="12"/>
+      <c r="M29" s="9"/>
       <c r="N29" s="1"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="27"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="18"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="12"/>
+      <c r="S29" s="9"/>
       <c r="T29" s="1"/>
       <c r="U29" s="3"/>
-      <c r="V29" s="12"/>
+      <c r="V29" s="9"/>
       <c r="W29" s="1"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="12"/>
+      <c r="X29" s="21"/>
+      <c r="Y29" s="9"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="1"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="12"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="1"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="12"/>
+      <c r="G30" s="9"/>
       <c r="H30" s="1"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="12"/>
+      <c r="J30" s="9"/>
       <c r="K30" s="1"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="12"/>
+      <c r="M30" s="9"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="36"/>
-      <c r="P30" s="33"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="24"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="12"/>
+      <c r="S30" s="9"/>
       <c r="T30" s="1"/>
       <c r="U30" s="3"/>
-      <c r="V30" s="12"/>
+      <c r="V30" s="9"/>
       <c r="W30" s="1"/>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="12"/>
+      <c r="X30" s="21"/>
+      <c r="Y30" s="9"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="1"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="12"/>
+      <c r="D31" s="9"/>
       <c r="E31" s="1"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="12"/>
+      <c r="G31" s="9"/>
       <c r="H31" s="1"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="12"/>
+      <c r="J31" s="9"/>
       <c r="K31" s="1"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="12"/>
+      <c r="M31" s="9"/>
       <c r="N31" s="1"/>
       <c r="O31" s="3"/>
-      <c r="P31" s="12"/>
+      <c r="P31" s="9"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="12"/>
+      <c r="S31" s="9"/>
       <c r="T31" s="1"/>
       <c r="U31" s="3"/>
-      <c r="V31" s="12"/>
+      <c r="V31" s="9"/>
       <c r="W31" s="1"/>
-      <c r="X31" s="30"/>
-      <c r="Y31" s="12"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="9"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="1"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="12"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="1"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="12"/>
+      <c r="G32" s="9"/>
       <c r="H32" s="1"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="12"/>
+      <c r="J32" s="9"/>
       <c r="K32" s="1"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="12"/>
+      <c r="M32" s="9"/>
       <c r="N32" s="1"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="12"/>
+      <c r="P32" s="9"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="3"/>
-      <c r="S32" s="12"/>
+      <c r="S32" s="9"/>
       <c r="T32" s="1"/>
       <c r="U32" s="3"/>
-      <c r="V32" s="12"/>
+      <c r="V32" s="9"/>
       <c r="W32" s="1"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="12"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="9"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="1"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="12"/>
+      <c r="D33" s="9"/>
       <c r="E33" s="1"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="12"/>
+      <c r="G33" s="9"/>
       <c r="H33" s="1"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="12"/>
+      <c r="J33" s="9"/>
       <c r="K33" s="1"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="12"/>
+      <c r="M33" s="9"/>
       <c r="N33" s="1"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="12"/>
+      <c r="P33" s="9"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="12"/>
+      <c r="S33" s="9"/>
       <c r="T33" s="1"/>
       <c r="U33" s="3"/>
-      <c r="V33" s="12"/>
+      <c r="V33" s="9"/>
       <c r="W33" s="1"/>
-      <c r="X33" s="30"/>
-      <c r="Y33" s="12"/>
+      <c r="X33" s="21"/>
+      <c r="Y33" s="9"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="12"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="1"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="12"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="1"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="12"/>
+      <c r="J34" s="9"/>
       <c r="K34" s="1"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="12"/>
+      <c r="M34" s="9"/>
       <c r="N34" s="1"/>
       <c r="O34" s="3"/>
-      <c r="P34" s="12"/>
+      <c r="P34" s="9"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="3"/>
-      <c r="S34" s="12"/>
+      <c r="S34" s="9"/>
       <c r="T34" s="1"/>
       <c r="U34" s="3"/>
-      <c r="V34" s="12"/>
+      <c r="V34" s="9"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="12"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="9"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="12"/>
+      <c r="D35" s="9"/>
       <c r="E35" s="1"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="9"/>
       <c r="H35" s="1"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="12"/>
+      <c r="J35" s="9"/>
       <c r="K35" s="1"/>
       <c r="L35" s="3"/>
-      <c r="M35" s="12"/>
+      <c r="M35" s="9"/>
       <c r="N35" s="1"/>
       <c r="O35" s="3"/>
-      <c r="P35" s="12"/>
+      <c r="P35" s="9"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="3"/>
-      <c r="S35" s="12"/>
+      <c r="S35" s="9"/>
       <c r="T35" s="1"/>
       <c r="U35" s="3"/>
-      <c r="V35" s="12"/>
+      <c r="V35" s="9"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="12"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="9"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="12"/>
+      <c r="D36" s="9"/>
       <c r="E36" s="1"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="9"/>
       <c r="H36" s="1"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="12"/>
+      <c r="J36" s="9"/>
       <c r="K36" s="1"/>
       <c r="L36" s="3"/>
-      <c r="M36" s="12"/>
+      <c r="M36" s="9"/>
       <c r="N36" s="1"/>
       <c r="O36" s="3"/>
-      <c r="P36" s="12"/>
+      <c r="P36" s="9"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="12"/>
+      <c r="S36" s="9"/>
       <c r="T36" s="1"/>
       <c r="U36" s="3"/>
-      <c r="V36" s="12"/>
+      <c r="V36" s="9"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="12"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="9"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="12"/>
+      <c r="D37" s="9"/>
       <c r="E37" s="1"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="12"/>
+      <c r="G37" s="9"/>
       <c r="H37" s="1"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="12"/>
+      <c r="J37" s="9"/>
       <c r="K37" s="1"/>
       <c r="L37" s="3"/>
-      <c r="M37" s="12"/>
+      <c r="M37" s="9"/>
       <c r="N37" s="1"/>
       <c r="O37" s="3"/>
-      <c r="P37" s="12"/>
+      <c r="P37" s="9"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="3"/>
-      <c r="S37" s="12"/>
+      <c r="S37" s="9"/>
       <c r="T37" s="1"/>
       <c r="U37" s="3"/>
-      <c r="V37" s="12"/>
+      <c r="V37" s="9"/>
       <c r="W37" s="1"/>
-      <c r="X37" s="30"/>
-      <c r="Y37" s="12"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="9"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="12"/>
+      <c r="D38" s="9"/>
       <c r="E38" s="1"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="12"/>
+      <c r="G38" s="9"/>
       <c r="H38" s="1"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="12"/>
+      <c r="J38" s="9"/>
       <c r="K38" s="1"/>
       <c r="L38" s="3"/>
-      <c r="M38" s="12"/>
+      <c r="M38" s="9"/>
       <c r="N38" s="1"/>
       <c r="O38" s="3"/>
-      <c r="P38" s="12"/>
+      <c r="P38" s="9"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="3"/>
-      <c r="S38" s="12"/>
+      <c r="S38" s="9"/>
       <c r="T38" s="1"/>
       <c r="U38" s="3"/>
-      <c r="V38" s="12"/>
+      <c r="V38" s="9"/>
       <c r="W38" s="1"/>
-      <c r="X38" s="30"/>
-      <c r="Y38" s="12"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="9"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="12"/>
+      <c r="D39" s="9"/>
       <c r="E39" s="1"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="12"/>
+      <c r="G39" s="9"/>
       <c r="H39" s="1"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="12"/>
+      <c r="J39" s="9"/>
       <c r="K39" s="1"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="12"/>
+      <c r="M39" s="9"/>
       <c r="N39" s="1"/>
       <c r="O39" s="3"/>
-      <c r="P39" s="12"/>
+      <c r="P39" s="9"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="12"/>
+      <c r="S39" s="9"/>
       <c r="T39" s="1"/>
       <c r="U39" s="3"/>
-      <c r="V39" s="12"/>
+      <c r="V39" s="9"/>
       <c r="W39" s="1"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="12"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="9"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="12"/>
+      <c r="D40" s="9"/>
       <c r="E40" s="1"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="12"/>
+      <c r="G40" s="9"/>
       <c r="H40" s="1"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="12"/>
+      <c r="J40" s="9"/>
       <c r="K40" s="1"/>
       <c r="L40" s="3"/>
-      <c r="M40" s="12"/>
+      <c r="M40" s="9"/>
       <c r="N40" s="1"/>
       <c r="O40" s="3"/>
-      <c r="P40" s="12"/>
+      <c r="P40" s="9"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="12"/>
+      <c r="S40" s="9"/>
       <c r="T40" s="1"/>
       <c r="U40" s="3"/>
-      <c r="V40" s="12"/>
+      <c r="V40" s="9"/>
       <c r="W40" s="1"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="12"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="9"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="12"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="1"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="12"/>
+      <c r="G41" s="9"/>
       <c r="H41" s="1"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="12"/>
+      <c r="J41" s="9"/>
       <c r="K41" s="1"/>
       <c r="L41" s="3"/>
-      <c r="M41" s="12"/>
+      <c r="M41" s="9"/>
       <c r="N41" s="1"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="12"/>
+      <c r="P41" s="9"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="3"/>
-      <c r="S41" s="12"/>
+      <c r="S41" s="9"/>
       <c r="T41" s="1"/>
       <c r="U41" s="3"/>
-      <c r="V41" s="12"/>
+      <c r="V41" s="9"/>
       <c r="W41" s="1"/>
-      <c r="X41" s="30"/>
-      <c r="Y41" s="12"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="9"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="12"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="1"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="12"/>
+      <c r="G42" s="9"/>
       <c r="H42" s="1"/>
       <c r="I42" s="3"/>
-      <c r="J42" s="12"/>
+      <c r="J42" s="9"/>
       <c r="K42" s="1"/>
       <c r="L42" s="3"/>
-      <c r="M42" s="12"/>
+      <c r="M42" s="9"/>
       <c r="N42" s="1"/>
       <c r="O42" s="3"/>
-      <c r="P42" s="12"/>
+      <c r="P42" s="9"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="3"/>
-      <c r="S42" s="12"/>
+      <c r="S42" s="9"/>
       <c r="T42" s="1"/>
       <c r="U42" s="3"/>
-      <c r="V42" s="12"/>
+      <c r="V42" s="9"/>
       <c r="W42" s="1"/>
-      <c r="X42" s="30"/>
-      <c r="Y42" s="12"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="9"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="12"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="1"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="12"/>
+      <c r="G43" s="9"/>
       <c r="H43" s="1"/>
       <c r="I43" s="3"/>
-      <c r="J43" s="12"/>
+      <c r="J43" s="9"/>
       <c r="K43" s="1"/>
       <c r="L43" s="3"/>
-      <c r="M43" s="12"/>
+      <c r="M43" s="9"/>
       <c r="N43" s="1"/>
       <c r="O43" s="3"/>
-      <c r="P43" s="12"/>
+      <c r="P43" s="9"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="3"/>
-      <c r="S43" s="12"/>
+      <c r="S43" s="9"/>
       <c r="T43" s="1"/>
       <c r="U43" s="3"/>
-      <c r="V43" s="12"/>
+      <c r="V43" s="9"/>
       <c r="W43" s="1"/>
-      <c r="X43" s="30"/>
-      <c r="Y43" s="12"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="9"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="12"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="1"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="12"/>
+      <c r="G44" s="9"/>
       <c r="H44" s="1"/>
       <c r="I44" s="3"/>
-      <c r="J44" s="12"/>
+      <c r="J44" s="9"/>
       <c r="K44" s="1"/>
       <c r="L44" s="3"/>
-      <c r="M44" s="12"/>
+      <c r="M44" s="9"/>
       <c r="N44" s="1"/>
       <c r="O44" s="3"/>
-      <c r="P44" s="12"/>
+      <c r="P44" s="9"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="3"/>
-      <c r="S44" s="12"/>
+      <c r="S44" s="9"/>
       <c r="T44" s="1"/>
       <c r="U44" s="3"/>
-      <c r="V44" s="12"/>
+      <c r="V44" s="9"/>
       <c r="W44" s="1"/>
-      <c r="X44" s="30"/>
-      <c r="Y44" s="12"/>
+      <c r="X44" s="21"/>
+      <c r="Y44" s="9"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="12"/>
+      <c r="D45" s="9"/>
       <c r="E45" s="1"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="12"/>
+      <c r="G45" s="9"/>
       <c r="H45" s="1"/>
       <c r="I45" s="3"/>
-      <c r="J45" s="12"/>
+      <c r="J45" s="9"/>
       <c r="K45" s="1"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="12"/>
+      <c r="M45" s="9"/>
       <c r="N45" s="1"/>
       <c r="O45" s="3"/>
-      <c r="P45" s="12"/>
+      <c r="P45" s="9"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="3"/>
-      <c r="S45" s="12"/>
+      <c r="S45" s="9"/>
       <c r="T45" s="1"/>
       <c r="U45" s="3"/>
-      <c r="V45" s="12"/>
+      <c r="V45" s="9"/>
       <c r="W45" s="1"/>
-      <c r="X45" s="30"/>
-      <c r="Y45" s="12"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="9"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="12"/>
+      <c r="D46" s="9"/>
       <c r="E46" s="1"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="12"/>
+      <c r="G46" s="9"/>
       <c r="H46" s="1"/>
       <c r="I46" s="3"/>
-      <c r="J46" s="12"/>
+      <c r="J46" s="9"/>
       <c r="K46" s="1"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="12"/>
+      <c r="M46" s="9"/>
       <c r="N46" s="1"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="12"/>
+      <c r="P46" s="9"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="3"/>
-      <c r="S46" s="12"/>
+      <c r="S46" s="9"/>
       <c r="T46" s="1"/>
       <c r="U46" s="3"/>
-      <c r="V46" s="12"/>
+      <c r="V46" s="9"/>
       <c r="W46" s="1"/>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="12"/>
+      <c r="X46" s="21"/>
+      <c r="Y46" s="9"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="12"/>
+      <c r="D47" s="9"/>
       <c r="E47" s="1"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="12"/>
+      <c r="G47" s="9"/>
       <c r="H47" s="1"/>
       <c r="I47" s="3"/>
-      <c r="J47" s="12"/>
+      <c r="J47" s="9"/>
       <c r="K47" s="1"/>
       <c r="L47" s="3"/>
-      <c r="M47" s="12"/>
+      <c r="M47" s="9"/>
       <c r="N47" s="1"/>
       <c r="O47" s="3"/>
-      <c r="P47" s="12"/>
+      <c r="P47" s="9"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="3"/>
-      <c r="S47" s="12"/>
+      <c r="S47" s="9"/>
       <c r="T47" s="1"/>
       <c r="U47" s="3"/>
-      <c r="V47" s="12"/>
+      <c r="V47" s="9"/>
       <c r="W47" s="1"/>
-      <c r="X47" s="30"/>
-      <c r="Y47" s="12"/>
+      <c r="X47" s="21"/>
+      <c r="Y47" s="9"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="12"/>
+      <c r="D48" s="9"/>
       <c r="E48" s="1"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="12"/>
+      <c r="G48" s="9"/>
       <c r="H48" s="1"/>
       <c r="I48" s="3"/>
-      <c r="J48" s="12"/>
+      <c r="J48" s="9"/>
       <c r="K48" s="1"/>
       <c r="L48" s="3"/>
-      <c r="M48" s="12"/>
+      <c r="M48" s="9"/>
       <c r="N48" s="1"/>
       <c r="O48" s="3"/>
-      <c r="P48" s="12"/>
+      <c r="P48" s="9"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="3"/>
-      <c r="S48" s="12"/>
+      <c r="S48" s="9"/>
       <c r="T48" s="1"/>
       <c r="U48" s="3"/>
-      <c r="V48" s="12"/>
+      <c r="V48" s="9"/>
       <c r="W48" s="1"/>
-      <c r="X48" s="30"/>
-      <c r="Y48" s="12"/>
+      <c r="X48" s="21"/>
+      <c r="Y48" s="9"/>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="12"/>
+      <c r="D49" s="9"/>
       <c r="E49" s="1"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="12"/>
+      <c r="G49" s="9"/>
       <c r="H49" s="1"/>
       <c r="I49" s="3"/>
-      <c r="J49" s="12"/>
+      <c r="J49" s="9"/>
       <c r="K49" s="1"/>
       <c r="L49" s="3"/>
-      <c r="M49" s="12"/>
+      <c r="M49" s="9"/>
       <c r="N49" s="1"/>
       <c r="O49" s="3"/>
-      <c r="P49" s="12"/>
+      <c r="P49" s="9"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="3"/>
-      <c r="S49" s="12"/>
+      <c r="S49" s="9"/>
       <c r="T49" s="1"/>
       <c r="U49" s="3"/>
-      <c r="V49" s="12"/>
+      <c r="V49" s="9"/>
       <c r="W49" s="1"/>
-      <c r="X49" s="30"/>
-      <c r="Y49" s="12"/>
+      <c r="X49" s="21"/>
+      <c r="Y49" s="9"/>
     </row>
     <row r="50" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="2"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="13"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="2"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="13"/>
+      <c r="G50" s="10"/>
       <c r="H50" s="2"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="13"/>
+      <c r="J50" s="10"/>
       <c r="K50" s="2"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="13"/>
+      <c r="M50" s="10"/>
       <c r="N50" s="2"/>
       <c r="O50" s="4"/>
-      <c r="P50" s="13"/>
+      <c r="P50" s="10"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="4"/>
-      <c r="S50" s="13"/>
+      <c r="S50" s="10"/>
       <c r="T50" s="2"/>
       <c r="U50" s="4"/>
-      <c r="V50" s="13"/>
+      <c r="V50" s="10"/>
       <c r="W50" s="2"/>
-      <c r="X50" s="32"/>
-      <c r="Y50" s="13"/>
+      <c r="X50" s="23"/>
+      <c r="Y50" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="O14:O17"/>
-    <mergeCell ref="P14:P17"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="R21:R23"/>
-    <mergeCell ref="S21:S23"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="U5:U10"/>
-    <mergeCell ref="V5:V10"/>
-    <mergeCell ref="O4:O6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
+  <mergeCells count="48">
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="R4:R6"/>
@@ -3825,6 +3789,44 @@
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="U5:U10"/>
+    <mergeCell ref="V5:V10"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="R21:R23"/>
+    <mergeCell ref="S21:S23"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="O14:O17"/>
+    <mergeCell ref="P14:P17"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout de tout les monstre en jeu reparti par map
</commit_message>
<xml_diff>
--- a/sources/Outiles/MobMap/AllMobe.xlsx
+++ b/sources/Outiles/MobMap/AllMobe.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat_wfpn4na\Documents\GitHub\Jeu-Dzarian-Miniquoinquoin\sources\Outiles\MobMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4EED30-1F54-4D95-BA41-5E50A19487A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{106410F2-8532-4655-A70F-15FCB742237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="21600" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="2520" windowWidth="21600" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="names" sheetId="1" r:id="rId1"/>
+    <sheet name="AllMobe" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="104">
   <si>
     <t>Amalgam_Sprite</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>HugeSlug_Sprite</t>
-  </si>
-  <si>
-    <t>BOSS_COMMUN</t>
   </si>
   <si>
     <t>HyperBot_Sprite</t>
@@ -1106,7 +1103,19 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1115,29 +1124,17 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1497,10 +1494,10 @@
   <dimension ref="A1:BQ50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V25" sqref="V25"/>
+      <selection pane="bottomRight" activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,46 +1530,46 @@
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="34" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="34" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="34" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="34" t="s">
+      <c r="L1" s="27"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="35"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="34" t="s">
+      <c r="O1" s="27"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="35"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="34" t="s">
+      <c r="R1" s="27"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="35"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="36"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="28"/>
     </row>
     <row r="2" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
@@ -1698,10 +1695,10 @@
       <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="36">
         <v>1</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="35" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1750,16 +1747,16 @@
         <v>3</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="U3" s="32">
+        <v>90</v>
+      </c>
+      <c r="U3" s="36">
         <v>1</v>
       </c>
-      <c r="V3" s="33" t="s">
+      <c r="V3" s="35" t="s">
         <v>3</v>
       </c>
       <c r="W3" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X3" s="20">
         <v>1</v>
@@ -1815,10 +1812,10 @@
     <row r="4" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="29"/>
+        <v>74</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1838,37 +1835,37 @@
         <v>7</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L4" s="26">
+        <v>93</v>
+      </c>
+      <c r="L4" s="29">
         <v>1</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="32" t="s">
         <v>3</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O4" s="26">
+        <v>75</v>
+      </c>
+      <c r="O4" s="29">
         <v>1</v>
       </c>
-      <c r="P4" s="28" t="s">
+      <c r="P4" s="32" t="s">
         <v>3</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R4" s="26">
+        <v>77</v>
+      </c>
+      <c r="R4" s="29">
         <v>1</v>
       </c>
-      <c r="S4" s="28" t="s">
+      <c r="S4" s="32" t="s">
         <v>3</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="27"/>
-      <c r="V4" s="29"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="34"/>
       <c r="W4" s="1"/>
       <c r="X4" s="21"/>
       <c r="Y4" s="9"/>
@@ -1920,7 +1917,7 @@
     <row r="5" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
@@ -1943,25 +1940,25 @@
       <c r="K5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="29"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="34"/>
       <c r="N5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O5" s="30"/>
-      <c r="P5" s="31"/>
+      <c r="P5" s="33"/>
       <c r="Q5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R5" s="30"/>
-      <c r="S5" s="31"/>
+      <c r="S5" s="33"/>
       <c r="T5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U5" s="26">
+      <c r="U5" s="29">
         <v>1</v>
       </c>
-      <c r="V5" s="28" t="s">
+      <c r="V5" s="32" t="s">
         <v>3</v>
       </c>
       <c r="W5" s="1"/>
@@ -2015,7 +2012,7 @@
     <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -2033,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I6" s="3">
         <v>2</v>
@@ -2045,20 +2042,20 @@
       <c r="L6" s="3"/>
       <c r="M6" s="9"/>
       <c r="N6" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="O6" s="27"/>
-      <c r="P6" s="29"/>
+        <v>100</v>
+      </c>
+      <c r="O6" s="31"/>
+      <c r="P6" s="34"/>
       <c r="Q6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="27"/>
-      <c r="S6" s="29"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="34"/>
       <c r="T6" s="12" t="s">
         <v>49</v>
       </c>
       <c r="U6" s="30"/>
-      <c r="V6" s="31"/>
+      <c r="V6" s="33"/>
       <c r="W6" s="12"/>
       <c r="X6" s="22"/>
       <c r="Y6" s="24"/>
@@ -2110,7 +2107,7 @@
     <row r="7" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -2131,7 +2128,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="9"/>
       <c r="K7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L7" s="3">
         <v>1</v>
@@ -2151,17 +2148,17 @@
       <c r="Q7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="26">
+      <c r="R7" s="29">
         <v>2</v>
       </c>
-      <c r="S7" s="28" t="s">
+      <c r="S7" s="32" t="s">
         <v>3</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="U7" s="30"/>
-      <c r="V7" s="31"/>
+      <c r="V7" s="33"/>
       <c r="W7" s="1"/>
       <c r="X7" s="22"/>
       <c r="Y7" s="24"/>
@@ -2216,12 +2213,12 @@
       <c r="C8" s="3"/>
       <c r="D8" s="9"/>
       <c r="E8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="26">
+        <v>84</v>
+      </c>
+      <c r="F8" s="29">
         <v>1</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="32" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="1"/>
@@ -2240,15 +2237,15 @@
         <v>2</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R8" s="27"/>
-      <c r="S8" s="29"/>
+        <v>67</v>
+      </c>
+      <c r="R8" s="31"/>
+      <c r="S8" s="34"/>
       <c r="T8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="U8" s="30"/>
-      <c r="V8" s="31"/>
+      <c r="V8" s="33"/>
       <c r="W8" s="1"/>
       <c r="X8" s="22"/>
       <c r="Y8" s="24"/>
@@ -2303,20 +2300,20 @@
       <c r="C9" s="3"/>
       <c r="D9" s="9"/>
       <c r="E9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="29"/>
+        <v>94</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="1"/>
       <c r="I9" s="3"/>
       <c r="J9" s="9"/>
       <c r="K9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L9" s="26">
+        <v>87</v>
+      </c>
+      <c r="L9" s="29">
         <v>1</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="32" t="s">
         <v>3</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -2332,10 +2329,10 @@
       <c r="R9" s="3"/>
       <c r="S9" s="9"/>
       <c r="T9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U9" s="30"/>
-      <c r="V9" s="31"/>
+      <c r="V9" s="33"/>
       <c r="W9" s="1"/>
       <c r="X9" s="21"/>
       <c r="Y9" s="9"/>
@@ -2395,17 +2392,17 @@
       <c r="H10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="29">
         <v>2</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="32" t="s">
         <v>3</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="27"/>
-      <c r="M10" s="29"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="34"/>
       <c r="N10" s="1" t="s">
         <v>47</v>
       </c>
@@ -2419,10 +2416,10 @@
       <c r="R10" s="3"/>
       <c r="S10" s="9"/>
       <c r="T10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="U10" s="27"/>
-      <c r="V10" s="29"/>
+        <v>81</v>
+      </c>
+      <c r="U10" s="31"/>
+      <c r="V10" s="34"/>
       <c r="W10" s="1"/>
       <c r="X10" s="21"/>
       <c r="Y10" s="9"/>
@@ -2474,27 +2471,27 @@
     <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="26">
+        <v>72</v>
+      </c>
+      <c r="C11" s="29">
         <v>1</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="3"/>
       <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" s="30"/>
-      <c r="J11" s="31"/>
+      <c r="J11" s="33"/>
       <c r="K11" s="1"/>
       <c r="L11" s="3"/>
       <c r="M11" s="9"/>
       <c r="N11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O11" s="3">
         <v>2</v>
@@ -2561,32 +2558,32 @@
       <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="29"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="29"/>
+        <v>70</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" s="26">
+        <v>96</v>
+      </c>
+      <c r="L12" s="29">
         <v>2</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="32" t="s">
         <v>3</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O12" s="26">
+        <v>92</v>
+      </c>
+      <c r="O12" s="29">
         <v>1</v>
       </c>
-      <c r="P12" s="28" t="s">
+      <c r="P12" s="32" t="s">
         <v>3</v>
       </c>
       <c r="Q12" s="1"/>
@@ -2611,25 +2608,25 @@
       <c r="I13" s="3"/>
       <c r="J13" s="9"/>
       <c r="K13" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L13" s="30"/>
-      <c r="M13" s="31"/>
+      <c r="M13" s="33"/>
       <c r="N13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="O13" s="27"/>
-      <c r="P13" s="29"/>
+        <v>86</v>
+      </c>
+      <c r="O13" s="31"/>
+      <c r="P13" s="34"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="3"/>
       <c r="S13" s="9"/>
       <c r="T13" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="U13" s="26">
+        <v>97</v>
+      </c>
+      <c r="U13" s="29">
         <v>1</v>
       </c>
-      <c r="V13" s="28" t="s">
+      <c r="V13" s="32" t="s">
         <v>3</v>
       </c>
       <c r="W13" s="1"/>
@@ -2648,27 +2645,27 @@
       <c r="I14" s="3"/>
       <c r="J14" s="9"/>
       <c r="K14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L14" s="27"/>
-      <c r="M14" s="29"/>
+        <v>98</v>
+      </c>
+      <c r="L14" s="31"/>
+      <c r="M14" s="34"/>
       <c r="N14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O14" s="26">
+        <v>95</v>
+      </c>
+      <c r="O14" s="29">
         <v>1</v>
       </c>
-      <c r="P14" s="28" t="s">
+      <c r="P14" s="32" t="s">
         <v>7</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="3"/>
       <c r="S14" s="9"/>
       <c r="T14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="U14" s="27"/>
-      <c r="V14" s="29"/>
+        <v>101</v>
+      </c>
+      <c r="U14" s="31"/>
+      <c r="V14" s="34"/>
       <c r="W14" s="1"/>
       <c r="X14" s="21"/>
       <c r="Y14" s="9"/>
@@ -2688,17 +2685,17 @@
       <c r="L15" s="3"/>
       <c r="M15" s="9"/>
       <c r="N15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O15" s="30"/>
-      <c r="P15" s="31"/>
+      <c r="P15" s="33"/>
       <c r="Q15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R15" s="26">
+        <v>66</v>
+      </c>
+      <c r="R15" s="29">
         <v>2</v>
       </c>
-      <c r="S15" s="28" t="s">
+      <c r="S15" s="32" t="s">
         <v>3</v>
       </c>
       <c r="T15" s="1"/>
@@ -2726,12 +2723,12 @@
         <v>21</v>
       </c>
       <c r="O16" s="30"/>
-      <c r="P16" s="31"/>
+      <c r="P16" s="33"/>
       <c r="Q16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="27"/>
-      <c r="S16" s="29"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="34"/>
       <c r="T16" s="1"/>
       <c r="U16" s="3"/>
       <c r="V16" s="9"/>
@@ -2754,10 +2751,10 @@
       <c r="L17" s="3"/>
       <c r="M17" s="9"/>
       <c r="N17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="O17" s="27"/>
-      <c r="P17" s="29"/>
+        <v>80</v>
+      </c>
+      <c r="O17" s="31"/>
+      <c r="P17" s="34"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="3"/>
       <c r="S17" s="9"/>
@@ -2783,13 +2780,13 @@
       <c r="L18" s="3"/>
       <c r="M18" s="9"/>
       <c r="N18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O18" s="29">
+        <v>2</v>
+      </c>
+      <c r="P18" s="32" t="s">
         <v>79</v>
-      </c>
-      <c r="O18" s="26">
-        <v>2</v>
-      </c>
-      <c r="P18" s="28" t="s">
-        <v>80</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="3"/>
@@ -2818,8 +2815,8 @@
       <c r="N19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="27"/>
-      <c r="P19" s="29"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="34"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="3"/>
       <c r="S19" s="9"/>
@@ -2842,22 +2839,22 @@
         <v>36</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F20" s="3">
         <v>3</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I20" s="3">
         <v>3</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>32</v>
@@ -2887,7 +2884,7 @@
         <v>4</v>
       </c>
       <c r="V20" s="9" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="W20" s="1"/>
       <c r="X20" s="21"/>
@@ -2923,22 +2920,22 @@
         <v>36</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="R21" s="26">
+        <v>76</v>
+      </c>
+      <c r="R21" s="29">
         <v>3</v>
       </c>
-      <c r="S21" s="28" t="s">
-        <v>64</v>
+      <c r="S21" s="32" t="s">
+        <v>63</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U21" s="3">
         <v>3</v>
       </c>
       <c r="V21" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W21" s="1"/>
       <c r="X21" s="21"/>
@@ -2947,7 +2944,7 @@
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="3">
         <v>3</v>
@@ -2965,7 +2962,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="9"/>
       <c r="N22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O22" s="3">
         <v>4</v>
@@ -2974,10 +2971,10 @@
         <v>36</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R22" s="30"/>
-      <c r="S22" s="31"/>
+      <c r="S22" s="33"/>
       <c r="T22" s="1"/>
       <c r="U22" s="3"/>
       <c r="V22" s="9"/>
@@ -2988,13 +2985,13 @@
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="29">
+        <v>3</v>
+      </c>
+      <c r="D23" s="32" t="s">
         <v>63</v>
-      </c>
-      <c r="C23" s="26">
-        <v>3</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>64</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="3"/>
@@ -3006,19 +3003,19 @@
       <c r="L23" s="3"/>
       <c r="M23" s="9"/>
       <c r="N23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O23" s="3">
         <v>5</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R23" s="27"/>
-      <c r="S23" s="29"/>
+        <v>85</v>
+      </c>
+      <c r="R23" s="31"/>
+      <c r="S23" s="34"/>
       <c r="T23" s="1"/>
       <c r="U23" s="3"/>
       <c r="V23" s="9"/>
@@ -3029,10 +3026,10 @@
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="29"/>
+        <v>102</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="9"/>
@@ -3043,22 +3040,22 @@
       <c r="L24" s="3"/>
       <c r="M24" s="9"/>
       <c r="N24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O24" s="3">
         <v>3</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R24" s="3">
         <v>2</v>
       </c>
       <c r="S24" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T24" s="1"/>
       <c r="U24" s="3"/>
@@ -3082,12 +3079,12 @@
       <c r="L25" s="3"/>
       <c r="M25" s="9"/>
       <c r="N25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O25" s="26">
+        <v>56</v>
+      </c>
+      <c r="O25" s="29">
         <v>3</v>
       </c>
-      <c r="P25" s="28" t="s">
+      <c r="P25" s="32" t="s">
         <v>36</v>
       </c>
       <c r="Q25" s="1"/>
@@ -3117,8 +3114,8 @@
       <c r="N26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="27"/>
-      <c r="P26" s="29"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="34"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="3"/>
       <c r="S26" s="9"/>
@@ -3779,6 +3776,39 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="R21:R23"/>
+    <mergeCell ref="S21:S23"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="O14:O17"/>
+    <mergeCell ref="P14:P17"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="U5:U10"/>
+    <mergeCell ref="V5:V10"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="R4:R6"/>
@@ -3790,43 +3820,10 @@
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="V3:V4"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="U5:U10"/>
-    <mergeCell ref="V5:V10"/>
-    <mergeCell ref="O4:O6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="R21:R23"/>
-    <mergeCell ref="S21:S23"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="O14:O17"/>
-    <mergeCell ref="P14:P17"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout des fichier csv map
</commit_message>
<xml_diff>
--- a/sources/Outiles/MobMap/AllMobe.xlsx
+++ b/sources/Outiles/MobMap/AllMobe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat_wfpn4na\Documents\GitHub\Jeu-Dzarian-Miniquoinquoin\sources\Outiles\MobMap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\code\GitHub\SpaceShooter\sources\Outiles\MobMap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{106410F2-8532-4655-A70F-15FCB742237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5B7A64-9AAE-4DBA-B836-1875261FDB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="2520" windowWidth="21600" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42375" yWindow="7380" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllMobe" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
   <si>
     <t>Amalgam_Sprite</t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>Plant42_Sprite</t>
-  </si>
-  <si>
-    <t>SHOOTER_STILL</t>
   </si>
   <si>
     <t>ProtoBot_Sprite</t>
@@ -1103,6 +1100,27 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1112,28 +1130,7 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1494,10 +1491,10 @@
   <dimension ref="A1:BQ50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V20" sqref="V20"/>
+      <selection pane="bottomRight" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,46 +1527,46 @@
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="26" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="26" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="26" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="26" t="s">
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="26" t="s">
+      <c r="O1" s="34"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="26" t="s">
+      <c r="R1" s="34"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="27"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="26" t="s">
+      <c r="U1" s="34"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="28"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="35"/>
     </row>
     <row r="2" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
@@ -1695,10 +1692,10 @@
       <c r="B3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="32">
         <v>1</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="36" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="13" t="s">
@@ -1747,12 +1744,12 @@
         <v>3</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="U3" s="36">
+        <v>89</v>
+      </c>
+      <c r="U3" s="32">
         <v>1</v>
       </c>
-      <c r="V3" s="35" t="s">
+      <c r="V3" s="36" t="s">
         <v>3</v>
       </c>
       <c r="W3" s="13" t="s">
@@ -1814,8 +1811,8 @@
       <c r="B4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="34"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1835,37 +1832,37 @@
         <v>7</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L4" s="29">
+        <v>92</v>
+      </c>
+      <c r="L4" s="26">
         <v>1</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="26">
         <v>1</v>
       </c>
-      <c r="P4" s="32" t="s">
+      <c r="P4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="R4" s="29">
+      <c r="R4" s="26">
         <v>1</v>
       </c>
-      <c r="S4" s="32" t="s">
+      <c r="S4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="31"/>
-      <c r="V4" s="34"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="29"/>
       <c r="W4" s="1"/>
       <c r="X4" s="21"/>
       <c r="Y4" s="9"/>
@@ -1940,25 +1937,25 @@
       <c r="K5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="34"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="29"/>
       <c r="N5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O5" s="30"/>
-      <c r="P5" s="33"/>
+      <c r="P5" s="31"/>
       <c r="Q5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R5" s="30"/>
-      <c r="S5" s="33"/>
+      <c r="S5" s="31"/>
       <c r="T5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U5" s="29">
+      <c r="U5" s="26">
         <v>1</v>
       </c>
-      <c r="V5" s="32" t="s">
+      <c r="V5" s="28" t="s">
         <v>3</v>
       </c>
       <c r="W5" s="1"/>
@@ -2012,7 +2009,7 @@
     <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -2042,20 +2039,20 @@
       <c r="L6" s="3"/>
       <c r="M6" s="9"/>
       <c r="N6" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="O6" s="31"/>
-      <c r="P6" s="34"/>
+        <v>99</v>
+      </c>
+      <c r="O6" s="27"/>
+      <c r="P6" s="29"/>
       <c r="Q6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="34"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="29"/>
       <c r="T6" s="12" t="s">
         <v>49</v>
       </c>
       <c r="U6" s="30"/>
-      <c r="V6" s="33"/>
+      <c r="V6" s="31"/>
       <c r="W6" s="12"/>
       <c r="X6" s="22"/>
       <c r="Y6" s="24"/>
@@ -2148,17 +2145,17 @@
       <c r="Q7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="29">
+      <c r="R7" s="26">
         <v>2</v>
       </c>
-      <c r="S7" s="32" t="s">
+      <c r="S7" s="28" t="s">
         <v>3</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="U7" s="30"/>
-      <c r="V7" s="33"/>
+      <c r="V7" s="31"/>
       <c r="W7" s="1"/>
       <c r="X7" s="22"/>
       <c r="Y7" s="24"/>
@@ -2213,12 +2210,12 @@
       <c r="C8" s="3"/>
       <c r="D8" s="9"/>
       <c r="E8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" s="29">
+        <v>83</v>
+      </c>
+      <c r="F8" s="26">
         <v>1</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="28" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="1"/>
@@ -2239,13 +2236,13 @@
       <c r="Q8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="34"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="29"/>
       <c r="T8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="U8" s="30"/>
-      <c r="V8" s="33"/>
+      <c r="V8" s="31"/>
       <c r="W8" s="1"/>
       <c r="X8" s="22"/>
       <c r="Y8" s="24"/>
@@ -2300,20 +2297,20 @@
       <c r="C9" s="3"/>
       <c r="D9" s="9"/>
       <c r="E9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="34"/>
+        <v>93</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="1"/>
       <c r="I9" s="3"/>
       <c r="J9" s="9"/>
       <c r="K9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L9" s="29">
+        <v>86</v>
+      </c>
+      <c r="L9" s="26">
         <v>1</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="28" t="s">
         <v>3</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -2332,7 +2329,7 @@
         <v>61</v>
       </c>
       <c r="U9" s="30"/>
-      <c r="V9" s="33"/>
+      <c r="V9" s="31"/>
       <c r="W9" s="1"/>
       <c r="X9" s="21"/>
       <c r="Y9" s="9"/>
@@ -2392,17 +2389,17 @@
       <c r="H10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="26">
         <v>2</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="28" t="s">
         <v>3</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="31"/>
-      <c r="M10" s="34"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="29"/>
       <c r="N10" s="1" t="s">
         <v>47</v>
       </c>
@@ -2416,10 +2413,10 @@
       <c r="R10" s="3"/>
       <c r="S10" s="9"/>
       <c r="T10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="U10" s="31"/>
-      <c r="V10" s="34"/>
+        <v>80</v>
+      </c>
+      <c r="U10" s="27"/>
+      <c r="V10" s="29"/>
       <c r="W10" s="1"/>
       <c r="X10" s="21"/>
       <c r="Y10" s="9"/>
@@ -2473,10 +2470,10 @@
       <c r="B11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="26">
         <v>1</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="28" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="1"/>
@@ -2486,7 +2483,7 @@
         <v>59</v>
       </c>
       <c r="I11" s="30"/>
-      <c r="J11" s="33"/>
+      <c r="J11" s="31"/>
       <c r="K11" s="1"/>
       <c r="L11" s="3"/>
       <c r="M11" s="9"/>
@@ -2558,32 +2555,32 @@
       <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="34"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="34"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="29"/>
       <c r="K12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L12" s="29">
+        <v>95</v>
+      </c>
+      <c r="L12" s="26">
         <v>2</v>
       </c>
-      <c r="M12" s="32" t="s">
+      <c r="M12" s="28" t="s">
         <v>3</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="O12" s="29">
+        <v>91</v>
+      </c>
+      <c r="O12" s="26">
         <v>1</v>
       </c>
-      <c r="P12" s="32" t="s">
+      <c r="P12" s="28" t="s">
         <v>3</v>
       </c>
       <c r="Q12" s="1"/>
@@ -2611,22 +2608,22 @@
         <v>58</v>
       </c>
       <c r="L13" s="30"/>
-      <c r="M13" s="33"/>
+      <c r="M13" s="31"/>
       <c r="N13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O13" s="31"/>
-      <c r="P13" s="34"/>
+        <v>85</v>
+      </c>
+      <c r="O13" s="27"/>
+      <c r="P13" s="29"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="3"/>
       <c r="S13" s="9"/>
       <c r="T13" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="U13" s="29">
+        <v>96</v>
+      </c>
+      <c r="U13" s="26">
         <v>1</v>
       </c>
-      <c r="V13" s="32" t="s">
+      <c r="V13" s="28" t="s">
         <v>3</v>
       </c>
       <c r="W13" s="1"/>
@@ -2645,27 +2642,27 @@
       <c r="I14" s="3"/>
       <c r="J14" s="9"/>
       <c r="K14" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L14" s="31"/>
-      <c r="M14" s="34"/>
+        <v>97</v>
+      </c>
+      <c r="L14" s="27"/>
+      <c r="M14" s="29"/>
       <c r="N14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O14" s="29">
+        <v>94</v>
+      </c>
+      <c r="O14" s="26">
         <v>1</v>
       </c>
-      <c r="P14" s="32" t="s">
+      <c r="P14" s="28" t="s">
         <v>7</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="3"/>
       <c r="S14" s="9"/>
       <c r="T14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="U14" s="31"/>
-      <c r="V14" s="34"/>
+        <v>100</v>
+      </c>
+      <c r="U14" s="27"/>
+      <c r="V14" s="29"/>
       <c r="W14" s="1"/>
       <c r="X14" s="21"/>
       <c r="Y14" s="9"/>
@@ -2688,14 +2685,14 @@
         <v>53</v>
       </c>
       <c r="O15" s="30"/>
-      <c r="P15" s="33"/>
+      <c r="P15" s="31"/>
       <c r="Q15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R15" s="29">
+      <c r="R15" s="26">
         <v>2</v>
       </c>
-      <c r="S15" s="32" t="s">
+      <c r="S15" s="28" t="s">
         <v>3</v>
       </c>
       <c r="T15" s="1"/>
@@ -2723,12 +2720,12 @@
         <v>21</v>
       </c>
       <c r="O16" s="30"/>
-      <c r="P16" s="33"/>
+      <c r="P16" s="31"/>
       <c r="Q16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="31"/>
-      <c r="S16" s="34"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="29"/>
       <c r="T16" s="1"/>
       <c r="U16" s="3"/>
       <c r="V16" s="9"/>
@@ -2751,10 +2748,10 @@
       <c r="L17" s="3"/>
       <c r="M17" s="9"/>
       <c r="N17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O17" s="31"/>
-      <c r="P17" s="34"/>
+        <v>79</v>
+      </c>
+      <c r="O17" s="27"/>
+      <c r="P17" s="29"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="3"/>
       <c r="S17" s="9"/>
@@ -2782,11 +2779,11 @@
       <c r="N18" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O18" s="29">
+      <c r="O18" s="26">
         <v>2</v>
       </c>
-      <c r="P18" s="32" t="s">
-        <v>79</v>
+      <c r="P18" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="3"/>
@@ -2815,8 +2812,8 @@
       <c r="N19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="31"/>
-      <c r="P19" s="34"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="29"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="3"/>
       <c r="S19" s="9"/>
@@ -2839,7 +2836,7 @@
         <v>36</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F20" s="3">
         <v>3</v>
@@ -2848,7 +2845,7 @@
         <v>63</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I20" s="3">
         <v>3</v>
@@ -2922,14 +2919,14 @@
       <c r="Q21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R21" s="29">
+      <c r="R21" s="26">
         <v>3</v>
       </c>
-      <c r="S21" s="32" t="s">
+      <c r="S21" s="28" t="s">
         <v>63</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U21" s="3">
         <v>3</v>
@@ -2971,10 +2968,10 @@
         <v>36</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R22" s="30"/>
-      <c r="S22" s="33"/>
+      <c r="S22" s="31"/>
       <c r="T22" s="1"/>
       <c r="U22" s="3"/>
       <c r="V22" s="9"/>
@@ -2987,10 +2984,10 @@
       <c r="B23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="26">
         <v>3</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="28" t="s">
         <v>63</v>
       </c>
       <c r="E23" s="1"/>
@@ -3012,10 +3009,10 @@
         <v>63</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="R23" s="31"/>
-      <c r="S23" s="34"/>
+        <v>84</v>
+      </c>
+      <c r="R23" s="27"/>
+      <c r="S23" s="29"/>
       <c r="T23" s="1"/>
       <c r="U23" s="3"/>
       <c r="V23" s="9"/>
@@ -3026,10 +3023,10 @@
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="9"/>
@@ -3049,7 +3046,7 @@
         <v>63</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R24" s="3">
         <v>2</v>
@@ -3081,10 +3078,10 @@
       <c r="N25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O25" s="29">
+      <c r="O25" s="26">
         <v>3</v>
       </c>
-      <c r="P25" s="32" t="s">
+      <c r="P25" s="28" t="s">
         <v>36</v>
       </c>
       <c r="Q25" s="1"/>
@@ -3114,8 +3111,8 @@
       <c r="N26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="31"/>
-      <c r="P26" s="34"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="29"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="3"/>
       <c r="S26" s="9"/>
@@ -3776,39 +3773,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="R21:R23"/>
-    <mergeCell ref="S21:S23"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="O14:O17"/>
-    <mergeCell ref="P14:P17"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="U5:U10"/>
-    <mergeCell ref="V5:V10"/>
-    <mergeCell ref="O4:O6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="R4:R6"/>
@@ -3824,6 +3788,39 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
+    <mergeCell ref="V5:V10"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="P14:P17"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="R21:R23"/>
+    <mergeCell ref="S21:S23"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="U5:U10"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="M12:M14"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="O14:O17"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>